<commit_message>
added files for AD simulation
</commit_message>
<xml_diff>
--- a/UpperRep/PowerAnalysisUpperRep.xlsx
+++ b/UpperRep/PowerAnalysisUpperRep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23955" windowHeight="12840"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9615" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Fall vs</t>
   </si>
@@ -40,54 +40,6 @@
   </si>
   <si>
     <t>Power</t>
-  </si>
-  <si>
-    <t>105-110</t>
-  </si>
-  <si>
-    <t>120-125</t>
-  </si>
-  <si>
-    <t>50-55</t>
-  </si>
-  <si>
-    <t>60-65</t>
-  </si>
-  <si>
-    <t>45-50</t>
-  </si>
-  <si>
-    <t>35-40</t>
-  </si>
-  <si>
-    <t>40-45</t>
-  </si>
-  <si>
-    <t>75-80</t>
-  </si>
-  <si>
-    <t>30-35</t>
-  </si>
-  <si>
-    <t>65-70</t>
-  </si>
-  <si>
-    <t>15-20</t>
-  </si>
-  <si>
-    <t>20-25</t>
-  </si>
-  <si>
-    <t>25-30</t>
-  </si>
-  <si>
-    <t>10-15.</t>
-  </si>
-  <si>
-    <t>95-100</t>
-  </si>
-  <si>
-    <t>160-165</t>
   </si>
 </sst>
 </file>
@@ -631,7 +583,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,6 +597,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -652,12 +607,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -997,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1011,13 +960,13 @@
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
@@ -1043,120 +992,120 @@
       <c r="A3" s="1">
         <v>0.5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7">
         <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>0.6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>21</v>
+      <c r="B4" s="2">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>0.7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="2">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2">
+        <v>68</v>
+      </c>
+      <c r="D5" s="2">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2">
         <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>0.8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
+      <c r="B6" s="2">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>0.9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
+      <c r="B7" s="2">
+        <v>102</v>
+      </c>
+      <c r="C7" s="2">
+        <v>103</v>
+      </c>
+      <c r="D7" s="2">
+        <v>55</v>
+      </c>
+      <c r="E7" s="2">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>0.99</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
+      <c r="B8" s="2">
+        <v>160</v>
+      </c>
+      <c r="C8" s="2">
+        <v>165</v>
+      </c>
+      <c r="D8" s="2">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2">
+        <v>56</v>
+      </c>
+      <c r="F8" s="2">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1170,13 +1119,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="16384" width="12.5703125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>73</v>
+      </c>
+      <c r="C3" s="2">
+        <v>72</v>
+      </c>
+      <c r="D3" s="2">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2">
+        <v>25</v>
+      </c>
+      <c r="F3" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2">
+        <v>84</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>97</v>
+      </c>
+      <c r="C5" s="2">
+        <v>98</v>
+      </c>
+      <c r="D5" s="2">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>113</v>
+      </c>
+      <c r="C6" s="2">
+        <v>114</v>
+      </c>
+      <c r="D6" s="2">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>138</v>
+      </c>
+      <c r="C7" s="2">
+        <v>139</v>
+      </c>
+      <c r="D7" s="2">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2">
+        <v>47</v>
+      </c>
+      <c r="F7" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="B8" s="2">
+        <v>203</v>
+      </c>
+      <c r="C8" s="2">
+        <v>211</v>
+      </c>
+      <c r="D8" s="2">
+        <v>106</v>
+      </c>
+      <c r="E8" s="2">
+        <v>69</v>
+      </c>
+      <c r="F8" s="2">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>